<commit_message>
update curve-convolution, fix button in processingtab
</commit_message>
<xml_diff>
--- a/Wi-UI.Tung.xlsx
+++ b/Wi-UI.Tung.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents_local\Workspace\WellInsight\wi-angular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Github\wi-angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,10 @@
     <sheet name="WorkingBlock" sheetId="10" r:id="rId10"/>
     <sheet name="Dialogs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="352">
   <si>
     <t>Code</t>
   </si>
@@ -1101,7 +1101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1294,8 +1294,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1637,7 +1665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1709,9 +1737,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="RibbonBlock!A1" display="RibbonBlock" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" location="ExplorerBlock!A1" display="ExplorerBlock" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" location="WorkingBlock!A1" display="WorkingBlock" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" location="RibbonBlock!A1" display="RibbonBlock"/>
+    <hyperlink ref="B3" location="ExplorerBlock!A1" display="ExplorerBlock"/>
+    <hyperlink ref="B4" location="WorkingBlock!A1" display="WorkingBlock"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1719,7 +1747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
@@ -2157,7 +2185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -3260,7 +3288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3363,12 +3391,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" location="ProjectTab!A1" display="ProjectTab" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B4" location="WellTab!A1" display="WellTab" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B5" location="DataAnalysisTab!A1" display="DataAnalysisTab" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B6" location="DataProcessingTab!A1" display="DataProcessingTab" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="B7" location="PetrophysicsTab!A1" display="PetrophysicsTab" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="B8" location="HelpTab!A1" display="HelpTab" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B3" location="ProjectTab!A1" display="ProjectTab"/>
+    <hyperlink ref="B4" location="WellTab!A1" display="WellTab"/>
+    <hyperlink ref="B5" location="DataAnalysisTab!A1" display="DataAnalysisTab"/>
+    <hyperlink ref="B6" location="DataProcessingTab!A1" display="DataProcessingTab"/>
+    <hyperlink ref="B7" location="PetrophysicsTab!A1" display="PetrophysicsTab"/>
+    <hyperlink ref="B8" location="HelpTab!A1" display="HelpTab"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3376,7 +3404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
@@ -3994,10 +4022,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -5380,11 +5408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7991,11 +8019,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8235,9 +8263,8 @@
       <c r="K6" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="L6" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>fix-btn-sm</v>
+      <c r="L6" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -8275,9 +8302,8 @@
       <c r="K7" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="L7" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>fix-btn-sm</v>
+      <c r="L7" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -8315,9 +8341,8 @@
       <c r="K8" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="L8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>fix-btn-sm</v>
+      <c r="L8" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -8396,9 +8421,8 @@
       <c r="K10" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="L10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>fix-btn-sm</v>
+      <c r="L10" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -8436,9 +8460,8 @@
       <c r="K11" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="L11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>fix-btn-sm</v>
+      <c r="L11" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -9723,7 +9746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
@@ -11110,7 +11133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -11410,7 +11433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
1 commit for new branch share-project
</commit_message>
<xml_diff>
--- a/Wi-UI.Tung.xlsx
+++ b/Wi-UI.Tung.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/revoltech/wi-angular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\wi-angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22920" windowHeight="14380" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22920" windowHeight="14385" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,10 @@
     <sheet name="WorkingBlock" sheetId="10" r:id="rId10"/>
     <sheet name="Dialogs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="362">
   <si>
     <t>Code</t>
   </si>
@@ -1123,12 +1123,15 @@
   </si>
   <si>
     <t>DataProcessing</t>
+  </si>
+  <si>
+    <t>Share Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1314,6 +1317,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1588,9 +1594,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1667,12 +1673,12 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1713,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -1800,7 +1806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>2.1</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>2.2000000000000002</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2.2999999999999998</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>3</v>
       </c>
@@ -1959,9 +1965,9 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>356</v>
       </c>
@@ -1972,14 +1978,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>SUBSTITUTE(CONCATENATE(B3,"Modal")," ","")</f>
         <v>NewProjectModal</v>
@@ -1991,7 +1997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>SUBSTITUTE(CONCATENATE(B4,"Modal")," ","")</f>
         <v>OpenProjectModal</v>
@@ -2003,7 +2009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>SUBSTITUTE(CONCATENATE(B5,"Modal")," ","")</f>
         <v>CloseProjectModal</v>
@@ -2018,7 +2024,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>SUBSTITUTE(CONCATENATE(B6,"Modal")," ","")</f>
         <v>UnitSettingsModal</v>
@@ -2030,7 +2036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>SUBSTITUTE(CONCATENATE(B7,"Modal")," ","")</f>
         <v>ExitModal</v>
@@ -2045,14 +2051,14 @@
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" ref="A9:A30" si="0">SUBSTITUTE(CONCATENATE(B9,"Modal")," ","")</f>
         <v>AddNewModal</v>
@@ -2061,7 +2067,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>WellHeaderModal</v>
@@ -2070,7 +2076,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>DepthConversionModal</v>
@@ -2079,7 +2085,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>CurveAliasModal</v>
@@ -2088,7 +2094,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>FamilyEditModal</v>
@@ -2097,7 +2103,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Input/OutputModal</v>
@@ -2106,7 +2112,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>ImportASCIIModal</v>
@@ -2115,7 +2121,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>ImportMultiASCIIModal</v>
@@ -2124,7 +2130,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>ImportLASModal</v>
@@ -2133,7 +2139,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>ImportMultiLASModal</v>
@@ -2142,7 +2148,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Interval/CoreLoaderModal</v>
@@ -2151,7 +2157,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Multi-wellCoreLoaderModal</v>
@@ -2160,7 +2166,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>ImportWellHeaderModal</v>
@@ -2169,7 +2175,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>ImportWellTopModal</v>
@@ -2178,7 +2184,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>ExportASCIIModal</v>
@@ -2187,7 +2193,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>ExportMultiASCIIModal</v>
@@ -2196,7 +2202,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>ExportLASModal</v>
@@ -2205,7 +2211,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>ExportMultiLASModal</v>
@@ -2214,7 +2220,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>ExportCoreDataModal</v>
@@ -2223,7 +2229,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Multi-wellCoreLoaderModal</v>
@@ -2232,7 +2238,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>ExportWellHeaderModal</v>
@@ -2241,7 +2247,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>ExportWellTopModal</v>
@@ -2250,14 +2256,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" ref="A32:A65" si="1">SUBSTITUTE(CONCATENATE(B32,"Modal")," ","")</f>
         <v>BlankLogplotModal</v>
@@ -2266,7 +2272,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="1"/>
         <v>TrippleComboModal</v>
@@ -2275,7 +2281,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="1"/>
         <v>DensityNeutronModal</v>
@@ -2284,7 +2290,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="1"/>
         <v>ResistivitySonicModal</v>
@@ -2293,7 +2299,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="1"/>
         <v>3TracksBlankModal</v>
@@ -2302,7 +2308,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="1"/>
         <v>InputCurveModal</v>
@@ -2311,7 +2317,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="1"/>
         <v>Litho+Syn.CurveModal</v>
@@ -2320,7 +2326,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="1"/>
         <v>Syn.CurveModal</v>
@@ -2329,7 +2335,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="1"/>
         <v>CrossPlotModal</v>
@@ -2338,7 +2344,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="1"/>
         <v>BlankCrossPlotModal</v>
@@ -2347,7 +2353,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="1"/>
         <v>SonicPHI_TOTALModal</v>
@@ -2356,7 +2362,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="1"/>
         <v>NeutronDensityModal</v>
@@ -2365,7 +2371,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="1"/>
         <v>NeutronGammaModal</v>
@@ -2374,7 +2380,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="1"/>
         <v>SonicGammaModal</v>
@@ -2383,7 +2389,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="1"/>
         <v>NeuTronSonicModal</v>
@@ -2392,7 +2398,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="1"/>
         <v>DenityGammaModal</v>
@@ -2401,7 +2407,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="1"/>
         <v>NeuTronRtModal</v>
@@ -2410,7 +2416,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="1"/>
         <v>DensitySonicModal</v>
@@ -2419,7 +2425,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="1"/>
         <v>DensityRtModal</v>
@@ -2428,7 +2434,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="1"/>
         <v>SonicDensityModal</v>
@@ -2437,7 +2443,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="1"/>
         <v>SonicRtModal</v>
@@ -2446,7 +2452,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="1"/>
         <v>RtRx0Modal</v>
@@ -2455,7 +2461,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="1"/>
         <v>PickettModal</v>
@@ -2464,7 +2470,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="1"/>
         <v>HistogramModal</v>
@@ -2473,7 +2479,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="1"/>
         <v>BlankHistogramModal</v>
@@ -2482,7 +2488,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="1"/>
         <v>PHI_TOTALModal</v>
@@ -2491,7 +2497,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="1"/>
         <v>GammaRayModal</v>
@@ -2500,7 +2506,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="1"/>
         <v>NeutronModal</v>
@@ -2509,7 +2515,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="1"/>
         <v>DensityModal</v>
@@ -2518,7 +2524,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="1"/>
         <v>HistogramMoreModal</v>
@@ -2527,7 +2533,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="1"/>
         <v>SonicModal</v>
@@ -2536,7 +2542,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="1"/>
         <v>SallowResistivityModal</v>
@@ -2545,7 +2551,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="1"/>
         <v>DeepResistivityModal</v>
@@ -2554,7 +2560,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="1"/>
         <v>MSFLHistogramModal</v>
@@ -2563,14 +2569,14 @@
         <v>219</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>360</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" ref="A67:A93" si="2">SUBSTITUTE(CONCATENATE(B67,"Modal")," ","")</f>
         <v>AddCurveModal</v>
@@ -2579,7 +2585,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="2"/>
         <v>InteractiveCurveEditModal</v>
@@ -2588,7 +2594,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="2"/>
         <v>InteractiveBaselineShiftModal</v>
@@ -2597,7 +2603,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="2"/>
         <v>SplitCurveModal</v>
@@ -2606,7 +2612,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="2"/>
         <v>SplitCurvesModal</v>
@@ -2615,7 +2621,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="2"/>
         <v>InteractiveCurveSplitModal</v>
@@ -2624,7 +2630,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="2"/>
         <v>MergeCurvesModal</v>
@@ -2633,7 +2639,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="2"/>
         <v>CurvesHeaderModal</v>
@@ -2642,7 +2648,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="2"/>
         <v>FillDataGapsModal</v>
@@ -2651,7 +2657,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="2"/>
         <v>CurveFilterModal</v>
@@ -2660,7 +2666,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="2"/>
         <v>CurveConvolutionModal</v>
@@ -2669,7 +2675,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="2"/>
         <v>CurveDeconvolutionModal</v>
@@ -2678,7 +2684,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="2"/>
         <v>CurveDerivativeModal</v>
@@ -2687,7 +2693,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="2"/>
         <v>CurveRescaleModal</v>
@@ -2696,7 +2702,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="2"/>
         <v>CurveComrarisonModal</v>
@@ -2705,7 +2711,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="2"/>
         <v>CurveAverageModal</v>
@@ -2714,7 +2720,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="2"/>
         <v>FormationResistivityModal</v>
@@ -2723,7 +2729,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="2"/>
         <v>Badhole/Coal/SaltModal</v>
@@ -2732,7 +2738,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="2"/>
         <v>UserFormulaModal</v>
@@ -2741,7 +2747,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="2"/>
         <v>UserFormulaModal</v>
@@ -2750,7 +2756,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="2"/>
         <v>UserProgramModal</v>
@@ -2759,7 +2765,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="2"/>
         <v>PythonProgramModal</v>
@@ -2768,7 +2774,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="2"/>
         <v>CalculationModal</v>
@@ -2777,7 +2783,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" si="2"/>
         <v>TVDConversionModal</v>
@@ -2786,7 +2792,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="2"/>
         <v>PCAAnalysisModal</v>
@@ -2795,7 +2801,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="2"/>
         <v>Multi-LinearRegressionModal</v>
@@ -2804,7 +2810,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="2"/>
         <v>NeuralNetworkModal</v>
@@ -2813,14 +2819,14 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" ref="A95:A116" si="3">SUBSTITUTE(CONCATENATE(B95,"Modal")," ","")</f>
         <v>EditZonesModal</v>
@@ -2829,7 +2835,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="3"/>
         <v>InputCurvesModal</v>
@@ -2838,7 +2844,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="3"/>
         <v>InputFuidModal</v>
@@ -2847,7 +2853,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="3"/>
         <v>BuildMineralParametersModal</v>
@@ -2856,7 +2862,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="3"/>
         <v>InputMineralZonesModal</v>
@@ -2865,7 +2871,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="3"/>
         <v>Multi-MineralSolverModal</v>
@@ -2874,7 +2880,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="3"/>
         <v>ClayMineralsVolumeModal</v>
@@ -2883,7 +2889,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f t="shared" si="3"/>
         <v>Fracture-VugPorosityModal</v>
@@ -2892,7 +2898,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f t="shared" si="3"/>
         <v>OpenPorosityModal</v>
@@ -2901,7 +2907,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f t="shared" si="3"/>
         <v>SecondaryPorosityModal</v>
@@ -2910,7 +2916,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="3"/>
         <v>FracturePorosityModal</v>
@@ -2919,7 +2925,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f t="shared" si="3"/>
         <v>FilteringFractureModal</v>
@@ -2928,7 +2934,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f t="shared" si="3"/>
         <v>Micro&amp;MacroPorosityModal</v>
@@ -2937,7 +2943,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="3"/>
         <v>WaterSaturationModal</v>
@@ -2946,7 +2952,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="3"/>
         <v>PermeabilityModal</v>
@@ -2955,7 +2961,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="3"/>
         <v>CutoffandSummationModal</v>
@@ -2964,7 +2970,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="3"/>
         <v>FilteringModal</v>
@@ -2973,7 +2979,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="3"/>
         <v>ClasticModal</v>
@@ -2982,7 +2988,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="3"/>
         <v>BasicAnalysisModal</v>
@@ -2991,7 +2997,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f t="shared" si="3"/>
         <v>ClayVolumeModal</v>
@@ -3000,7 +3006,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f t="shared" si="3"/>
         <v>Porosity&amp;WaterSaturationModal</v>
@@ -3009,7 +3015,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="3"/>
         <v>CutoffandSummationModal</v>
@@ -3018,14 +3024,14 @@
         <v>331</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f>SUBSTITUTE(CONCATENATE(B118,"Modal")," ","")</f>
         <v>AboutModal</v>
@@ -3034,7 +3040,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f>SUBSTITUTE(CONCATENATE(B119,"Modal")," ","")</f>
         <v>UnlockModal</v>
@@ -3057,9 +3063,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3085,7 +3091,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -3096,7 +3102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.2</v>
       </c>
@@ -3107,7 +3113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1.3</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1.4</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1.5</v>
       </c>
@@ -3140,7 +3146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1.6</v>
       </c>
@@ -3170,16 +3176,16 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3217,7 +3223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -3286,7 +3292,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.3</v>
       </c>
@@ -3366,7 +3372,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1.4</v>
       </c>
@@ -3406,7 +3412,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>43</v>
       </c>
@@ -3447,13 +3453,13 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>SaveProjectButton</v>
+        <f>SUBSTITUTE(CONCATENATE(G8,D8)," ","")</f>
+        <v>ShareProjectButton</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -3470,7 +3476,7 @@
         <v>save-16x16</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>361</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="3"/>
@@ -3486,7 +3492,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
@@ -3525,7 +3531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>53</v>
       </c>
@@ -3565,7 +3571,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>56</v>
       </c>
@@ -3605,7 +3611,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>2</v>
       </c>
@@ -3644,7 +3650,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2.1</v>
       </c>
@@ -3684,7 +3690,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2.2000000000000002</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -3762,7 +3768,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
@@ -3800,7 +3806,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>72</v>
       </c>
@@ -3840,7 +3846,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3</v>
       </c>
@@ -3876,7 +3882,7 @@
       </c>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>3.1</v>
       </c>
@@ -3930,12 +3936,12 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="8.83203125" style="19"/>
+    <col min="10" max="10" width="8.85546875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3973,7 +3979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -4042,7 +4048,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.2</v>
       </c>
@@ -4082,7 +4088,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1.3</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1.4</v>
       </c>
@@ -4162,7 +4168,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1.5</v>
       </c>
@@ -4202,7 +4208,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>88</v>
       </c>
@@ -4237,7 +4243,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>2.1</v>
       </c>
@@ -4278,7 +4284,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>91</v>
       </c>
@@ -4317,7 +4323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>94</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>96</v>
       </c>
@@ -4395,7 +4401,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>99</v>
       </c>
@@ -4434,7 +4440,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>101</v>
       </c>
@@ -4473,7 +4479,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>104</v>
       </c>
@@ -4512,7 +4518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>107</v>
       </c>
@@ -4551,7 +4557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>110</v>
       </c>
@@ -4590,7 +4596,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>112</v>
       </c>
@@ -4631,7 +4637,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>64</v>
       </c>
@@ -4670,7 +4676,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>68</v>
       </c>
@@ -4709,7 +4715,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>118</v>
       </c>
@@ -4748,7 +4754,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>121</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>123</v>
       </c>
@@ -4826,7 +4832,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>125</v>
       </c>
@@ -4865,7 +4871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>126</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>128</v>
       </c>
@@ -4957,12 +4963,12 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5000,7 +5006,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -5029,7 +5035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -5069,7 +5075,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -5109,7 +5115,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.3</v>
       </c>
@@ -5149,7 +5155,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1.4</v>
       </c>
@@ -5189,7 +5195,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1.5</v>
       </c>
@@ -5230,7 +5236,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -5269,7 +5275,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
@@ -5308,7 +5314,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>146</v>
       </c>
@@ -5347,7 +5353,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>149</v>
       </c>
@@ -5386,7 +5392,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>152</v>
       </c>
@@ -5425,7 +5431,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>2</v>
       </c>
@@ -5463,7 +5469,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>2.1</v>
       </c>
@@ -5503,7 +5509,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>2.2000000000000002</v>
       </c>
@@ -5543,7 +5549,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>2.2999999999999998</v>
       </c>
@@ -5583,7 +5589,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>2.4</v>
       </c>
@@ -5623,7 +5629,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>2.5</v>
       </c>
@@ -5663,7 +5669,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2.6</v>
       </c>
@@ -5704,7 +5710,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>167</v>
       </c>
@@ -5743,7 +5749,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>170</v>
       </c>
@@ -5782,7 +5788,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>172</v>
       </c>
@@ -5821,7 +5827,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>175</v>
       </c>
@@ -5860,7 +5866,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>178</v>
       </c>
@@ -5899,7 +5905,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>181</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>184</v>
       </c>
@@ -5977,7 +5983,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>187</v>
       </c>
@@ -6016,7 +6022,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>190</v>
       </c>
@@ -6055,7 +6061,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>3</v>
       </c>
@@ -6090,7 +6096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>194</v>
       </c>
@@ -6130,7 +6136,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>197</v>
       </c>
@@ -6170,7 +6176,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>200</v>
       </c>
@@ -6206,7 +6212,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>203</v>
       </c>
@@ -6246,7 +6252,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>206</v>
       </c>
@@ -6286,7 +6292,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>3.6</v>
       </c>
@@ -6327,7 +6333,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>211</v>
       </c>
@@ -6366,7 +6372,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>214</v>
       </c>
@@ -6405,7 +6411,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>217</v>
       </c>
@@ -6444,7 +6450,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -6455,7 +6461,7 @@
       <c r="H41" s="19"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
@@ -6466,7 +6472,7 @@
       <c r="H42" s="19"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -6477,7 +6483,7 @@
       <c r="H43" s="19"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
@@ -6488,7 +6494,7 @@
       <c r="H44" s="19"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
@@ -6499,7 +6505,7 @@
       <c r="H45" s="19"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
@@ -6510,7 +6516,7 @@
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
@@ -6521,7 +6527,7 @@
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
@@ -6532,7 +6538,7 @@
       <c r="H48" s="19"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
@@ -6543,7 +6549,7 @@
       <c r="H49" s="19"/>
       <c r="I49" s="19"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
@@ -6554,7 +6560,7 @@
       <c r="H50" s="19"/>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
@@ -6565,7 +6571,7 @@
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
@@ -6576,7 +6582,7 @@
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="22"/>
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
@@ -6587,7 +6593,7 @@
       <c r="H53" s="19"/>
       <c r="I53" s="19"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -6598,7 +6604,7 @@
       <c r="H54" s="19"/>
       <c r="I54" s="19"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
@@ -6609,7 +6615,7 @@
       <c r="H55" s="19"/>
       <c r="I55" s="19"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
@@ -6620,7 +6626,7 @@
       <c r="H56" s="19"/>
       <c r="I56" s="19"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
@@ -6631,7 +6637,7 @@
       <c r="H57" s="19"/>
       <c r="I57" s="19"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
@@ -6642,7 +6648,7 @@
       <c r="H58" s="19"/>
       <c r="I58" s="19"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
@@ -6653,7 +6659,7 @@
       <c r="H59" s="19"/>
       <c r="I59" s="19"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
       <c r="B60" s="19"/>
       <c r="C60" s="20"/>
@@ -6664,7 +6670,7 @@
       <c r="H60" s="19"/>
       <c r="I60" s="19"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
@@ -6675,7 +6681,7 @@
       <c r="H61" s="19"/>
       <c r="I61" s="19"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
       <c r="B62" s="19"/>
       <c r="C62" s="19"/>
@@ -6686,7 +6692,7 @@
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="22"/>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
@@ -6697,7 +6703,7 @@
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="22"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
@@ -6708,7 +6714,7 @@
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="22"/>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
@@ -6719,7 +6725,7 @@
       <c r="H65" s="19"/>
       <c r="I65" s="19"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
@@ -6730,7 +6736,7 @@
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>
@@ -6741,7 +6747,7 @@
       <c r="H67" s="19"/>
       <c r="I67" s="19"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
@@ -6752,7 +6758,7 @@
       <c r="H68" s="19"/>
       <c r="I68" s="19"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
@@ -6763,7 +6769,7 @@
       <c r="H69" s="19"/>
       <c r="I69" s="19"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
       <c r="B70" s="19"/>
       <c r="C70" s="20"/>
@@ -6774,7 +6780,7 @@
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
@@ -6785,7 +6791,7 @@
       <c r="H71" s="19"/>
       <c r="I71" s="19"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="22"/>
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
@@ -6796,7 +6802,7 @@
       <c r="H72" s="19"/>
       <c r="I72" s="19"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="22"/>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
@@ -6807,7 +6813,7 @@
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="22"/>
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
@@ -6818,7 +6824,7 @@
       <c r="H74" s="19"/>
       <c r="I74" s="19"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="22"/>
       <c r="B75" s="19"/>
       <c r="C75" s="19"/>
@@ -6829,7 +6835,7 @@
       <c r="H75" s="19"/>
       <c r="I75" s="19"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
       <c r="B76" s="19"/>
       <c r="C76" s="20"/>
@@ -6840,7 +6846,7 @@
       <c r="H76" s="19"/>
       <c r="I76" s="19"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="22"/>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
@@ -6851,7 +6857,7 @@
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="22"/>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
@@ -6862,7 +6868,7 @@
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
@@ -6873,7 +6879,7 @@
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
@@ -6884,7 +6890,7 @@
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
@@ -6895,7 +6901,7 @@
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
@@ -6906,7 +6912,7 @@
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
@@ -6917,7 +6923,7 @@
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
@@ -6928,7 +6934,7 @@
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
@@ -6939,7 +6945,7 @@
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -6950,7 +6956,7 @@
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
@@ -6961,7 +6967,7 @@
       <c r="H87" s="19"/>
       <c r="I87" s="19"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="22"/>
       <c r="B88" s="19"/>
       <c r="C88" s="19"/>
@@ -6972,7 +6978,7 @@
       <c r="H88" s="19"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="22"/>
       <c r="B89" s="19"/>
       <c r="C89" s="19"/>
@@ -6983,7 +6989,7 @@
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="22"/>
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
@@ -6994,7 +7000,7 @@
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="22"/>
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
@@ -7005,7 +7011,7 @@
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
       <c r="B92" s="19"/>
       <c r="C92" s="19"/>
@@ -7016,7 +7022,7 @@
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="22"/>
       <c r="B93" s="19"/>
       <c r="C93" s="19"/>
@@ -7027,7 +7033,7 @@
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="22"/>
       <c r="B94" s="19"/>
       <c r="C94" s="19"/>
@@ -7038,7 +7044,7 @@
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="22"/>
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
@@ -7049,7 +7055,7 @@
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="22"/>
       <c r="B96" s="19"/>
       <c r="C96" s="19"/>
@@ -7060,7 +7066,7 @@
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
       <c r="B97" s="19"/>
       <c r="C97" s="19"/>
@@ -7071,7 +7077,7 @@
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="22"/>
       <c r="B98" s="19"/>
       <c r="C98" s="19"/>
@@ -7082,7 +7088,7 @@
       <c r="H98" s="19"/>
       <c r="I98" s="19"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="22"/>
       <c r="B99" s="19"/>
       <c r="C99" s="19"/>
@@ -7093,7 +7099,7 @@
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="22"/>
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
@@ -7104,7 +7110,7 @@
       <c r="H100" s="19"/>
       <c r="I100" s="19"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="22"/>
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
@@ -7115,7 +7121,7 @@
       <c r="H101" s="19"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="22"/>
       <c r="B102" s="19"/>
       <c r="C102" s="19"/>
@@ -7126,7 +7132,7 @@
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="22"/>
       <c r="B103" s="19"/>
       <c r="C103" s="19"/>
@@ -7137,7 +7143,7 @@
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="22"/>
       <c r="B104" s="19"/>
       <c r="C104" s="19"/>
@@ -7148,7 +7154,7 @@
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="22"/>
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
@@ -7159,7 +7165,7 @@
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="22"/>
       <c r="B106" s="19"/>
       <c r="C106" s="19"/>
@@ -7170,7 +7176,7 @@
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="22"/>
       <c r="B107" s="19"/>
       <c r="C107" s="19"/>
@@ -7181,7 +7187,7 @@
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="22"/>
       <c r="B108" s="19"/>
       <c r="C108" s="19"/>
@@ -7192,7 +7198,7 @@
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
       <c r="B109" s="19"/>
       <c r="C109" s="19"/>
@@ -7203,7 +7209,7 @@
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="22"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
@@ -7214,7 +7220,7 @@
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="22"/>
       <c r="B111" s="19"/>
       <c r="C111" s="19"/>
@@ -7225,7 +7231,7 @@
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="22"/>
       <c r="B112" s="19"/>
       <c r="C112" s="19"/>
@@ -7236,7 +7242,7 @@
       <c r="H112" s="19"/>
       <c r="I112" s="19"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="22"/>
       <c r="B113" s="19"/>
       <c r="C113" s="19"/>
@@ -7247,7 +7253,7 @@
       <c r="H113" s="19"/>
       <c r="I113" s="19"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="22"/>
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
@@ -7258,7 +7264,7 @@
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="22"/>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
@@ -7269,7 +7275,7 @@
       <c r="H115" s="19"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="22"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
@@ -7280,7 +7286,7 @@
       <c r="H116" s="19"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
@@ -7291,7 +7297,7 @@
       <c r="H117" s="19"/>
       <c r="I117" s="19"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="22"/>
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
@@ -7302,205 +7308,205 @@
       <c r="H118" s="19"/>
       <c r="I118" s="19"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D119" t="str">
         <f t="shared" ref="D119:D152" si="7">REPLACE(C119, 1, 2, "")</f>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D120" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D121" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D122" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D123" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D124" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D125" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D126" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D127" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D128" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D140" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D141" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D142" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D143" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D144" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D149" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -7520,12 +7526,12 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7563,7 +7569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -7595,7 +7601,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>222</v>
       </c>
@@ -7635,7 +7641,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>225</v>
       </c>
@@ -7675,7 +7681,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>228</v>
       </c>
@@ -7716,7 +7722,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>231</v>
       </c>
@@ -7755,7 +7761,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>233</v>
       </c>
@@ -7794,7 +7800,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>236</v>
       </c>
@@ -7833,7 +7839,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>239</v>
       </c>
@@ -7874,7 +7880,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>242</v>
       </c>
@@ -7913,7 +7919,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>245</v>
       </c>
@@ -7952,7 +7958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -7992,7 +7998,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
@@ -8032,7 +8038,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>56</v>
       </c>
@@ -8072,7 +8078,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>254</v>
       </c>
@@ -8112,7 +8118,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>257</v>
       </c>
@@ -8152,7 +8158,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>260</v>
       </c>
@@ -8192,7 +8198,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>263</v>
       </c>
@@ -8232,7 +8238,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>266</v>
       </c>
@@ -8272,7 +8278,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>269</v>
       </c>
@@ -8312,7 +8318,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>272</v>
       </c>
@@ -8352,7 +8358,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>275</v>
       </c>
@@ -8392,7 +8398,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>278</v>
       </c>
@@ -8432,7 +8438,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>88</v>
       </c>
@@ -8468,7 +8474,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>283</v>
       </c>
@@ -8508,7 +8514,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>112</v>
       </c>
@@ -8548,7 +8554,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>71</v>
       </c>
@@ -8588,7 +8594,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>289</v>
       </c>
@@ -8624,7 +8630,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>194</v>
       </c>
@@ -8664,7 +8670,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>197</v>
       </c>
@@ -8704,7 +8710,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>200</v>
       </c>
@@ -8744,7 +8750,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>203</v>
       </c>
@@ -8798,12 +8804,12 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -8841,7 +8847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -8873,7 +8879,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -8913,7 +8919,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -8953,7 +8959,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.3</v>
       </c>
@@ -8993,7 +8999,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1.4</v>
       </c>
@@ -9033,7 +9039,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>1.5</v>
       </c>
@@ -9073,7 +9079,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1.6</v>
       </c>
@@ -9113,7 +9119,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>1.7</v>
       </c>
@@ -9153,7 +9159,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1.8</v>
       </c>
@@ -9193,7 +9199,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>1.9</v>
       </c>
@@ -9233,7 +9239,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>260</v>
       </c>
@@ -9273,7 +9279,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>263</v>
       </c>
@@ -9313,7 +9319,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>266</v>
       </c>
@@ -9353,7 +9359,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>269</v>
       </c>
@@ -9393,7 +9399,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>272</v>
       </c>
@@ -9433,7 +9439,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>275</v>
       </c>
@@ -9473,7 +9479,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>278</v>
       </c>
@@ -9513,7 +9519,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>332</v>
       </c>
@@ -9553,7 +9559,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>2</v>
       </c>
@@ -9589,7 +9595,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>2.1</v>
       </c>
@@ -9629,7 +9635,7 @@
         <v>height65</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>2.2000000000000002</v>
       </c>
@@ -9669,7 +9675,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>2.2999999999999998</v>
       </c>
@@ -9709,7 +9715,7 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>2.4</v>
       </c>
@@ -9749,21 +9755,21 @@
         <v>fix-btn-sm</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="H25" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="H26" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -9781,7 +9787,7 @@
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -9799,7 +9805,7 @@
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="25"/>
       <c r="C29" s="19"/>
@@ -9817,7 +9823,7 @@
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="25"/>
       <c r="C30" s="19"/>
@@ -9835,7 +9841,7 @@
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="25"/>
       <c r="C31" s="19"/>
@@ -9853,7 +9859,7 @@
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="25"/>
       <c r="C32" s="19"/>
@@ -9871,7 +9877,7 @@
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="25"/>
       <c r="C33" s="19"/>
@@ -9889,7 +9895,7 @@
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="25"/>
       <c r="C34" s="19"/>
@@ -9907,7 +9913,7 @@
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="25"/>
       <c r="C35" s="19"/>
@@ -9925,7 +9931,7 @@
       <c r="L35" s="19"/>
       <c r="M35" s="19"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="25"/>
       <c r="C36" s="19"/>
@@ -9957,12 +9963,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -10000,7 +10006,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -10029,7 +10035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>222</v>
       </c>
@@ -10068,7 +10074,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -10107,7 +10113,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.3</v>
       </c>
@@ -10160,12 +10166,12 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -10200,7 +10206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -10229,7 +10235,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -10261,7 +10267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -10293,7 +10299,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -10325,7 +10331,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>2.1</v>
       </c>

</xml_diff>